<commit_message>
Added summaries at the top to reference important metrics
</commit_message>
<xml_diff>
--- a/Bitcoin_Lightning_Bank_Yield_Estimate_Calculator.xlsx
+++ b/Bitcoin_Lightning_Bank_Yield_Estimate_Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/20eb409204932c1c/Lightning Bank Case Study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5976" documentId="13_ncr:1_{AE93A452-22DF-478B-8AAE-1A3A6016AB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCEFE72E-B6AC-4F22-8311-8DB5919C29B0}"/>
+  <xr:revisionPtr revIDLastSave="5986" documentId="13_ncr:1_{AE93A452-22DF-478B-8AAE-1A3A6016AB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94EB14B7-30D7-4FD4-A03D-265E8CBE7D0E}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{10396A79-A4B2-467C-A467-ECE59C587EB2}"/>
   </bookViews>
@@ -202,9 +202,6 @@
     <t>Lightning Bank Bitcoin Total Value Locked (TVL)</t>
   </si>
   <si>
-    <t>Yield Summary</t>
-  </si>
-  <si>
     <t>SB Total Summary</t>
   </si>
   <si>
@@ -239,9 +236,6 @@
 Pairing Bitcoin Investors with Fiat Investors for Yield Farming</t>
   </si>
   <si>
-    <t>Lightning Bank Bitcoin TVL Total Yield Summary</t>
-  </si>
-  <si>
     <t>Bitcoin Compound Annual Growth Rate Calculator</t>
   </si>
   <si>
@@ -268,6 +262,14 @@
   <si>
     <t>Test Case Annual Average USD</t>
   </si>
+  <si>
+    <t>Yield Estimate Summary
+Stable Receiver (SR), Stable Provider (SP), Stable Balancer (SB)</t>
+  </si>
+  <si>
+    <t>Yield Estimate Summary
+Lightning Bank Bitcoin TVL Totals</t>
+  </si>
 </sst>
 </file>
 
@@ -281,7 +283,7 @@
     <numFmt numFmtId="168" formatCode="#,##0,&quot; K&quot;"/>
     <numFmt numFmtId="169" formatCode="###0.0,,&quot; M&quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,14 +328,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="0"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Aptos Display"/>
       <family val="2"/>
@@ -421,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -698,11 +692,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -998,9 +1016,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="168" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1016,22 +1031,94 @@
     <xf numFmtId="3" fontId="4" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1046,91 +1133,25 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1545,49 +1566,49 @@
       <c r="M1" s="23"/>
       <c r="N1" s="23"/>
     </row>
-    <row r="2" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="23"/>
-      <c r="B2" s="105" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="111" t="s">
+      <c r="B2" s="128" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="129"/>
+      <c r="D2" s="134" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="112"/>
+      <c r="E2" s="135"/>
       <c r="F2" s="23"/>
-      <c r="G2" s="115" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
+      <c r="G2" s="142" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
       <c r="J2" s="28"/>
-      <c r="K2" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="54"/>
-      <c r="M2" s="99"/>
+      <c r="K2" s="143" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="144"/>
+      <c r="M2" s="144"/>
       <c r="N2" s="28"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="23"/>
-      <c r="B3" s="107"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="114"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="137"/>
       <c r="F3" s="23"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="113"/>
-      <c r="I3" s="113"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
       <c r="J3" s="28"/>
-      <c r="K3" s="100">
+      <c r="K3" s="99">
         <f>C160</f>
         <v>20000</v>
       </c>
       <c r="L3" s="69" t="s">
-        <v>63</v>
-      </c>
-      <c r="M3" s="102">
+        <v>62</v>
+      </c>
+      <c r="M3" s="101">
         <f>I185</f>
         <v>329.62622716725173</v>
       </c>
@@ -1596,8 +1617,8 @@
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="28"/>
-      <c r="B4" s="107"/>
-      <c r="C4" s="108"/>
+      <c r="B4" s="130"/>
+      <c r="C4" s="131"/>
       <c r="D4" s="69" t="s">
         <v>3</v>
       </c>
@@ -1606,7 +1627,7 @@
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="94" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H4" s="69" t="s">
         <v>36</v>
@@ -1616,14 +1637,14 @@
         <v>0.18</v>
       </c>
       <c r="J4" s="28"/>
-      <c r="K4" s="100">
+      <c r="K4" s="99">
         <f>C160</f>
         <v>20000</v>
       </c>
       <c r="L4" s="93" t="s">
-        <v>64</v>
-      </c>
-      <c r="M4" s="103">
+        <v>63</v>
+      </c>
+      <c r="M4" s="102">
         <f>I186</f>
         <v>1648.1311358362589</v>
       </c>
@@ -1632,17 +1653,17 @@
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="75"/>
-      <c r="B5" s="107"/>
-      <c r="C5" s="108"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="131"/>
       <c r="D5" s="47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="71">
         <v>0.01</v>
       </c>
       <c r="F5" s="75"/>
       <c r="G5" s="93" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" s="93" t="s">
         <v>36</v>
@@ -1652,12 +1673,12 @@
         <v>0.39404159999999999</v>
       </c>
       <c r="J5" s="75"/>
-      <c r="K5" s="100">
+      <c r="K5" s="99">
         <f>C163</f>
         <v>400000</v>
       </c>
       <c r="L5" s="69" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M5" s="60">
         <f>I188</f>
@@ -1668,8 +1689,8 @@
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="75"/>
-      <c r="B6" s="107"/>
-      <c r="C6" s="108"/>
+      <c r="B6" s="130"/>
+      <c r="C6" s="131"/>
       <c r="D6" s="47" t="s">
         <v>0</v>
       </c>
@@ -1678,7 +1699,7 @@
       </c>
       <c r="F6" s="75"/>
       <c r="G6" s="78" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="98" t="s">
         <v>34</v>
@@ -1688,14 +1709,14 @@
         <v>9.0000000000000011E-3</v>
       </c>
       <c r="J6" s="75"/>
-      <c r="K6" s="100">
+      <c r="K6" s="99">
         <f>C163</f>
         <v>400000</v>
       </c>
       <c r="L6" s="93" t="s">
-        <v>64</v>
-      </c>
-      <c r="M6" s="103">
+        <v>63</v>
+      </c>
+      <c r="M6" s="102">
         <f>I189</f>
         <v>32962.622716725178</v>
       </c>
@@ -1704,8 +1725,8 @@
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="28"/>
-      <c r="B7" s="107"/>
-      <c r="C7" s="108"/>
+      <c r="B7" s="130"/>
+      <c r="C7" s="131"/>
       <c r="D7" s="69" t="s">
         <v>4</v>
       </c>
@@ -1714,24 +1735,24 @@
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="93" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H7" s="91" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I7" s="96">
         <f>I58</f>
         <v>0.20758291199999998</v>
       </c>
       <c r="J7" s="28"/>
-      <c r="K7" s="101">
+      <c r="K7" s="100">
         <f>C190</f>
         <v>1000000</v>
       </c>
       <c r="L7" s="69" t="s">
-        <v>63</v>
-      </c>
-      <c r="M7" s="103">
+        <v>62</v>
+      </c>
+      <c r="M7" s="102">
         <f>I191</f>
         <v>16481.311358362585</v>
       </c>
@@ -1740,8 +1761,8 @@
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="28"/>
-      <c r="B8" s="107"/>
-      <c r="C8" s="108"/>
+      <c r="B8" s="130"/>
+      <c r="C8" s="131"/>
       <c r="D8" s="69" t="s">
         <v>5</v>
       </c>
@@ -1750,24 +1771,24 @@
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="91" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H8" s="91" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I8" s="96">
         <f>I63</f>
         <v>0.44244576000000002</v>
       </c>
       <c r="J8" s="28"/>
-      <c r="K8" s="101">
+      <c r="K8" s="100">
         <f>C166</f>
         <v>1000000</v>
       </c>
       <c r="L8" s="93" t="s">
-        <v>64</v>
-      </c>
-      <c r="M8" s="103">
+        <v>63</v>
+      </c>
+      <c r="M8" s="102">
         <f>I192</f>
         <v>82406.556791812953</v>
       </c>
@@ -1776,8 +1797,8 @@
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="28"/>
-      <c r="B9" s="107"/>
-      <c r="C9" s="108"/>
+      <c r="B9" s="130"/>
+      <c r="C9" s="131"/>
       <c r="D9" s="69" t="s">
         <v>6</v>
       </c>
@@ -1786,24 +1807,24 @@
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="91" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" s="91" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I9" s="96">
         <f>I98</f>
         <v>6.3984589754269044E-2</v>
       </c>
       <c r="J9" s="23"/>
-      <c r="K9" s="101">
+      <c r="K9" s="100">
         <f>C169</f>
         <v>2100000</v>
       </c>
       <c r="L9" s="69" t="s">
-        <v>63</v>
-      </c>
-      <c r="M9" s="104">
+        <v>62</v>
+      </c>
+      <c r="M9" s="103">
         <f>I194</f>
         <v>34610.753852561429</v>
       </c>
@@ -1812,8 +1833,8 @@
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="28"/>
-      <c r="B10" s="109"/>
-      <c r="C10" s="110"/>
+      <c r="B10" s="132"/>
+      <c r="C10" s="133"/>
       <c r="D10" s="69" t="s">
         <v>22</v>
       </c>
@@ -1823,24 +1844,24 @@
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="92" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H10" s="91" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I10" s="97">
         <f>I143</f>
         <v>3.6562622716725175E-2</v>
       </c>
       <c r="J10" s="23"/>
-      <c r="K10" s="101">
+      <c r="K10" s="100">
         <f>C169</f>
         <v>2100000</v>
       </c>
       <c r="L10" s="93" t="s">
-        <v>64</v>
-      </c>
-      <c r="M10" s="104">
+        <v>63</v>
+      </c>
+      <c r="M10" s="103">
         <f>I195</f>
         <v>173053.76926280718</v>
       </c>
@@ -1865,62 +1886,62 @@
       <c r="O11" s="23"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="111" t="s">
+      <c r="B12" s="134" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="54"/>
       <c r="D12" s="54"/>
-      <c r="E12" s="117" t="s">
+      <c r="E12" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="117" t="s">
+      <c r="F12" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="117" t="s">
+      <c r="G12" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="117" t="s">
+      <c r="H12" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="117" t="s">
+      <c r="I12" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="117" t="s">
+      <c r="J12" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="117" t="s">
+      <c r="K12" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="117" t="s">
+      <c r="L12" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="117" t="s">
+      <c r="M12" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="N12" s="117" t="s">
+      <c r="N12" s="118" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="113"/>
+      <c r="B13" s="136"/>
       <c r="C13" s="61"/>
       <c r="D13" s="61"/>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="118"/>
-      <c r="I13" s="118"/>
-      <c r="J13" s="118"/>
-      <c r="K13" s="118"/>
-      <c r="L13" s="118"/>
-      <c r="M13" s="118"/>
-      <c r="N13" s="118"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="119"/>
+      <c r="H13" s="119"/>
+      <c r="I13" s="119"/>
+      <c r="J13" s="119"/>
+      <c r="K13" s="119"/>
+      <c r="L13" s="119"/>
+      <c r="M13" s="119"/>
+      <c r="N13" s="119"/>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="129" t="s">
+      <c r="B14" s="110" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="129"/>
+      <c r="C14" s="110"/>
       <c r="D14" s="48" t="s">
         <v>45</v>
       </c>
@@ -1966,8 +1987,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="131"/>
-      <c r="C15" s="131"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="112"/>
       <c r="D15" s="48" t="s">
         <v>46</v>
       </c>
@@ -2013,10 +2034,10 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="129" t="s">
+      <c r="B16" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="130"/>
+      <c r="C16" s="111"/>
       <c r="D16" s="48" t="s">
         <v>35</v>
       </c>
@@ -2062,8 +2083,8 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="133"/>
-      <c r="C17" s="134"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="115"/>
       <c r="D17" s="48" t="s">
         <v>43</v>
       </c>
@@ -2109,8 +2130,8 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="133"/>
-      <c r="C18" s="134"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="115"/>
       <c r="D18" s="44" t="s">
         <v>34</v>
       </c>
@@ -2156,10 +2177,10 @@
       </c>
     </row>
     <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="131"/>
-      <c r="C19" s="132"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="113"/>
       <c r="D19" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E19" s="46"/>
       <c r="F19" s="46"/>
@@ -2179,10 +2200,10 @@
       </c>
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="129" t="s">
+      <c r="B20" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="130"/>
+      <c r="C20" s="111"/>
       <c r="D20" s="44" t="s">
         <v>51</v>
       </c>
@@ -2228,8 +2249,8 @@
       </c>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="131"/>
-      <c r="C21" s="132"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="113"/>
       <c r="D21" s="44" t="s">
         <v>52</v>
       </c>
@@ -2291,7 +2312,7 @@
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="23"/>
-      <c r="B23" s="135" t="s">
+      <c r="B23" s="116" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="79" t="s">
@@ -2301,40 +2322,40 @@
         <f>E7</f>
         <v>0.45</v>
       </c>
-      <c r="E23" s="117" t="s">
+      <c r="E23" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="117" t="s">
+      <c r="F23" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="117" t="s">
+      <c r="G23" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="117" t="s">
+      <c r="H23" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="I23" s="117" t="s">
+      <c r="I23" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="117" t="s">
+      <c r="J23" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="K23" s="117" t="s">
+      <c r="K23" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="L23" s="117" t="s">
+      <c r="L23" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="M23" s="117" t="s">
+      <c r="M23" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="N23" s="117" t="s">
+      <c r="N23" s="118" t="s">
         <v>16</v>
       </c>
       <c r="O23" s="23"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="136"/>
+      <c r="B24" s="117"/>
       <c r="C24" s="81" t="s">
         <v>50</v>
       </c>
@@ -2342,22 +2363,22 @@
         <f>"10 BTC / "&amp;TEXT($E$4*10, "$###0.00,,")&amp;"M USD"</f>
         <v>10 BTC / $1.00M USD</v>
       </c>
-      <c r="E24" s="118"/>
-      <c r="F24" s="118"/>
-      <c r="G24" s="118"/>
-      <c r="H24" s="118"/>
-      <c r="I24" s="118"/>
-      <c r="J24" s="118"/>
-      <c r="K24" s="118"/>
-      <c r="L24" s="118"/>
-      <c r="M24" s="118"/>
-      <c r="N24" s="118"/>
+      <c r="E24" s="119"/>
+      <c r="F24" s="119"/>
+      <c r="G24" s="119"/>
+      <c r="H24" s="119"/>
+      <c r="I24" s="119"/>
+      <c r="J24" s="119"/>
+      <c r="K24" s="119"/>
+      <c r="L24" s="119"/>
+      <c r="M24" s="119"/>
+      <c r="N24" s="119"/>
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="125" t="s">
+      <c r="B25" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="126" t="s">
+      <c r="C25" s="120" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="44" t="s">
@@ -2405,10 +2426,10 @@
       </c>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="125"/>
-      <c r="C26" s="126"/>
+      <c r="B26" s="121"/>
+      <c r="C26" s="120"/>
       <c r="D26" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E26" s="45"/>
       <c r="F26" s="45"/>
@@ -2428,8 +2449,8 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="125"/>
-      <c r="C27" s="126"/>
+      <c r="B27" s="121"/>
+      <c r="C27" s="120"/>
       <c r="D27" s="44" t="s">
         <v>35</v>
       </c>
@@ -2475,8 +2496,8 @@
       </c>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="125"/>
-      <c r="C28" s="125"/>
+      <c r="B28" s="121"/>
+      <c r="C28" s="121"/>
       <c r="D28" s="48" t="s">
         <v>37</v>
       </c>
@@ -2523,8 +2544,8 @@
       <c r="R28" s="40"/>
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="125"/>
-      <c r="C29" s="125"/>
+      <c r="B29" s="121"/>
+      <c r="C29" s="121"/>
       <c r="D29" s="48" t="s">
         <v>38</v>
       </c>
@@ -2571,8 +2592,8 @@
       <c r="R29" s="40"/>
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="125"/>
-      <c r="C30" s="126" t="s">
+      <c r="B30" s="121"/>
+      <c r="C30" s="120" t="s">
         <v>48</v>
       </c>
       <c r="D30" s="44" t="s">
@@ -2620,8 +2641,8 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="125"/>
-      <c r="C31" s="125"/>
+      <c r="B31" s="121"/>
+      <c r="C31" s="121"/>
       <c r="D31" s="48" t="s">
         <v>39</v>
       </c>
@@ -2667,8 +2688,8 @@
       </c>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="125"/>
-      <c r="C32" s="125"/>
+      <c r="B32" s="121"/>
+      <c r="C32" s="121"/>
       <c r="D32" s="48" t="s">
         <v>40</v>
       </c>
@@ -2714,8 +2735,8 @@
       </c>
     </row>
     <row r="33" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="125"/>
-      <c r="C33" s="126" t="s">
+      <c r="B33" s="121"/>
+      <c r="C33" s="120" t="s">
         <v>47</v>
       </c>
       <c r="D33" s="44" t="s">
@@ -2764,10 +2785,10 @@
       <c r="R33" s="43"/>
     </row>
     <row r="34" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="125"/>
-      <c r="C34" s="126"/>
+      <c r="B34" s="121"/>
+      <c r="C34" s="120"/>
       <c r="D34" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E34" s="46"/>
       <c r="F34" s="46"/>
@@ -2787,8 +2808,8 @@
       </c>
     </row>
     <row r="35" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="125"/>
-      <c r="C35" s="125"/>
+      <c r="B35" s="121"/>
+      <c r="C35" s="121"/>
       <c r="D35" s="48" t="s">
         <v>39</v>
       </c>
@@ -2834,10 +2855,10 @@
       </c>
     </row>
     <row r="36" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="125"/>
-      <c r="C36" s="125"/>
+      <c r="B36" s="121"/>
+      <c r="C36" s="121"/>
       <c r="D36" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E36" s="51"/>
       <c r="F36" s="51"/>
@@ -2857,8 +2878,8 @@
       </c>
     </row>
     <row r="37" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B37" s="125"/>
-      <c r="C37" s="125"/>
+      <c r="B37" s="121"/>
+      <c r="C37" s="121"/>
       <c r="D37" s="48" t="s">
         <v>40</v>
       </c>
@@ -2904,10 +2925,10 @@
       </c>
     </row>
     <row r="38" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="125" t="s">
+      <c r="B38" s="121" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="126" t="s">
+      <c r="C38" s="120" t="s">
         <v>31</v>
       </c>
       <c r="D38" s="44" t="s">
@@ -2956,8 +2977,8 @@
       <c r="R38" s="40"/>
     </row>
     <row r="39" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B39" s="125"/>
-      <c r="C39" s="126"/>
+      <c r="B39" s="121"/>
+      <c r="C39" s="120"/>
       <c r="D39" s="44" t="s">
         <v>35</v>
       </c>
@@ -3004,8 +3025,8 @@
       <c r="R39" s="40"/>
     </row>
     <row r="40" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="125"/>
-      <c r="C40" s="125"/>
+      <c r="B40" s="121"/>
+      <c r="C40" s="121"/>
       <c r="D40" s="48" t="s">
         <v>37</v>
       </c>
@@ -3051,8 +3072,8 @@
       </c>
     </row>
     <row r="41" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="125"/>
-      <c r="C41" s="125"/>
+      <c r="B41" s="121"/>
+      <c r="C41" s="121"/>
       <c r="D41" s="48" t="s">
         <v>38</v>
       </c>
@@ -3098,8 +3119,8 @@
       </c>
     </row>
     <row r="42" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="125"/>
-      <c r="C42" s="126" t="s">
+      <c r="B42" s="121"/>
+      <c r="C42" s="120" t="s">
         <v>48</v>
       </c>
       <c r="D42" s="44" t="s">
@@ -3148,10 +3169,10 @@
       <c r="R42" s="40"/>
     </row>
     <row r="43" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="125"/>
-      <c r="C43" s="126"/>
+      <c r="B43" s="121"/>
+      <c r="C43" s="120"/>
       <c r="D43" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E43" s="45"/>
       <c r="F43" s="45"/>
@@ -3172,8 +3193,8 @@
       <c r="R43" s="40"/>
     </row>
     <row r="44" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="125"/>
-      <c r="C44" s="125"/>
+      <c r="B44" s="121"/>
+      <c r="C44" s="121"/>
       <c r="D44" s="48" t="s">
         <v>39</v>
       </c>
@@ -3220,10 +3241,10 @@
       <c r="R44" s="40"/>
     </row>
     <row r="45" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="125"/>
-      <c r="C45" s="125"/>
+      <c r="B45" s="121"/>
+      <c r="C45" s="121"/>
       <c r="D45" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E45" s="53"/>
       <c r="F45" s="53"/>
@@ -3244,8 +3265,8 @@
       <c r="R45" s="40"/>
     </row>
     <row r="46" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="125"/>
-      <c r="C46" s="125"/>
+      <c r="B46" s="121"/>
+      <c r="C46" s="121"/>
       <c r="D46" s="48" t="s">
         <v>40</v>
       </c>
@@ -3292,8 +3313,8 @@
       <c r="R46" s="40"/>
     </row>
     <row r="47" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="125"/>
-      <c r="C47" s="126" t="s">
+      <c r="B47" s="121"/>
+      <c r="C47" s="120" t="s">
         <v>47</v>
       </c>
       <c r="D47" s="44" t="s">
@@ -3342,10 +3363,10 @@
       <c r="R47" s="40"/>
     </row>
     <row r="48" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="125"/>
-      <c r="C48" s="126"/>
+      <c r="B48" s="121"/>
+      <c r="C48" s="120"/>
       <c r="D48" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E48" s="46"/>
       <c r="F48" s="46"/>
@@ -3366,8 +3387,8 @@
       <c r="R48" s="40"/>
     </row>
     <row r="49" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="125"/>
-      <c r="C49" s="125"/>
+      <c r="B49" s="121"/>
+      <c r="C49" s="121"/>
       <c r="D49" s="48" t="s">
         <v>39</v>
       </c>
@@ -3414,10 +3435,10 @@
       <c r="R49" s="40"/>
     </row>
     <row r="50" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="125"/>
-      <c r="C50" s="125"/>
+      <c r="B50" s="121"/>
+      <c r="C50" s="121"/>
       <c r="D50" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E50" s="52"/>
       <c r="F50" s="52"/>
@@ -3438,8 +3459,8 @@
       <c r="R50" s="40"/>
     </row>
     <row r="51" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="125"/>
-      <c r="C51" s="125"/>
+      <c r="B51" s="121"/>
+      <c r="C51" s="121"/>
       <c r="D51" s="48" t="s">
         <v>40</v>
       </c>
@@ -3486,10 +3507,10 @@
       <c r="R51" s="40"/>
     </row>
     <row r="52" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="125" t="s">
+      <c r="B52" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="126" t="s">
+      <c r="C52" s="120" t="s">
         <v>31</v>
       </c>
       <c r="D52" s="44" t="s">
@@ -3537,10 +3558,10 @@
       </c>
     </row>
     <row r="53" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="125"/>
-      <c r="C53" s="126"/>
+      <c r="B53" s="121"/>
+      <c r="C53" s="120"/>
       <c r="D53" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E53" s="45"/>
       <c r="F53" s="45"/>
@@ -3560,8 +3581,8 @@
       </c>
     </row>
     <row r="54" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="125"/>
-      <c r="C54" s="126"/>
+      <c r="B54" s="121"/>
+      <c r="C54" s="120"/>
       <c r="D54" s="44" t="s">
         <v>35</v>
       </c>
@@ -3607,8 +3628,8 @@
       </c>
     </row>
     <row r="55" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B55" s="125"/>
-      <c r="C55" s="125"/>
+      <c r="B55" s="121"/>
+      <c r="C55" s="121"/>
       <c r="D55" s="48" t="s">
         <v>37</v>
       </c>
@@ -3654,8 +3675,8 @@
       </c>
     </row>
     <row r="56" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B56" s="125"/>
-      <c r="C56" s="125"/>
+      <c r="B56" s="121"/>
+      <c r="C56" s="121"/>
       <c r="D56" s="48" t="s">
         <v>38</v>
       </c>
@@ -3701,8 +3722,8 @@
       </c>
     </row>
     <row r="57" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="125"/>
-      <c r="C57" s="126" t="s">
+      <c r="B57" s="121"/>
+      <c r="C57" s="120" t="s">
         <v>48</v>
       </c>
       <c r="D57" s="44" t="s">
@@ -3750,10 +3771,10 @@
       </c>
     </row>
     <row r="58" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="125"/>
-      <c r="C58" s="126"/>
+      <c r="B58" s="121"/>
+      <c r="C58" s="120"/>
       <c r="D58" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E58" s="45"/>
       <c r="F58" s="45"/>
@@ -3773,8 +3794,8 @@
       </c>
     </row>
     <row r="59" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B59" s="125"/>
-      <c r="C59" s="125"/>
+      <c r="B59" s="121"/>
+      <c r="C59" s="121"/>
       <c r="D59" s="48" t="s">
         <v>39</v>
       </c>
@@ -3820,10 +3841,10 @@
       </c>
     </row>
     <row r="60" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B60" s="125"/>
-      <c r="C60" s="125"/>
+      <c r="B60" s="121"/>
+      <c r="C60" s="121"/>
       <c r="D60" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E60" s="50"/>
       <c r="F60" s="50"/>
@@ -3844,8 +3865,8 @@
       <c r="R60" s="40"/>
     </row>
     <row r="61" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="125"/>
-      <c r="C61" s="125"/>
+      <c r="B61" s="121"/>
+      <c r="C61" s="121"/>
       <c r="D61" s="48" t="s">
         <v>40</v>
       </c>
@@ -3891,8 +3912,8 @@
       </c>
     </row>
     <row r="62" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B62" s="125"/>
-      <c r="C62" s="126" t="s">
+      <c r="B62" s="121"/>
+      <c r="C62" s="120" t="s">
         <v>47</v>
       </c>
       <c r="D62" s="44" t="s">
@@ -3940,10 +3961,10 @@
       </c>
     </row>
     <row r="63" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B63" s="125"/>
-      <c r="C63" s="126"/>
+      <c r="B63" s="121"/>
+      <c r="C63" s="120"/>
       <c r="D63" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E63" s="46"/>
       <c r="F63" s="46"/>
@@ -3963,8 +3984,8 @@
       </c>
     </row>
     <row r="64" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B64" s="125"/>
-      <c r="C64" s="125"/>
+      <c r="B64" s="121"/>
+      <c r="C64" s="121"/>
       <c r="D64" s="48" t="s">
         <v>39</v>
       </c>
@@ -4010,10 +4031,10 @@
       </c>
     </row>
     <row r="65" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B65" s="125"/>
-      <c r="C65" s="125"/>
+      <c r="B65" s="121"/>
+      <c r="C65" s="121"/>
       <c r="D65" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E65" s="51"/>
       <c r="F65" s="51"/>
@@ -4034,8 +4055,8 @@
       <c r="R65" s="43"/>
     </row>
     <row r="66" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B66" s="125"/>
-      <c r="C66" s="125"/>
+      <c r="B66" s="121"/>
+      <c r="C66" s="121"/>
       <c r="D66" s="48" t="s">
         <v>40</v>
       </c>
@@ -4098,7 +4119,7 @@
       <c r="O67" s="23"/>
     </row>
     <row r="68" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B68" s="121" t="s">
+      <c r="B68" s="126" t="s">
         <v>19</v>
       </c>
       <c r="C68" s="82" t="s">
@@ -4108,39 +4129,39 @@
         <f>E8</f>
         <v>0.35</v>
       </c>
-      <c r="E68" s="117" t="s">
+      <c r="E68" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="F68" s="117" t="s">
+      <c r="F68" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="G68" s="117" t="s">
+      <c r="G68" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="H68" s="117" t="s">
+      <c r="H68" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="I68" s="117" t="s">
+      <c r="I68" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="J68" s="117" t="s">
+      <c r="J68" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="K68" s="117" t="s">
+      <c r="K68" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="L68" s="117" t="s">
+      <c r="L68" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="M68" s="117" t="s">
+      <c r="M68" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="N68" s="117" t="s">
+      <c r="N68" s="118" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B69" s="122"/>
+      <c r="B69" s="127"/>
       <c r="C69" s="84" t="s">
         <v>50</v>
       </c>
@@ -4148,22 +4169,22 @@
         <f>"10 BTC / "&amp;TEXT($E$4*10, "$###0.00,,")&amp;"M USD"</f>
         <v>10 BTC / $1.00M USD</v>
       </c>
-      <c r="E69" s="118"/>
-      <c r="F69" s="118"/>
-      <c r="G69" s="118"/>
-      <c r="H69" s="118"/>
-      <c r="I69" s="118"/>
-      <c r="J69" s="118"/>
-      <c r="K69" s="118"/>
-      <c r="L69" s="118"/>
-      <c r="M69" s="118"/>
-      <c r="N69" s="118"/>
+      <c r="E69" s="119"/>
+      <c r="F69" s="119"/>
+      <c r="G69" s="119"/>
+      <c r="H69" s="119"/>
+      <c r="I69" s="119"/>
+      <c r="J69" s="119"/>
+      <c r="K69" s="119"/>
+      <c r="L69" s="119"/>
+      <c r="M69" s="119"/>
+      <c r="N69" s="119"/>
     </row>
     <row r="70" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B70" s="125" t="s">
+      <c r="B70" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="C70" s="126" t="s">
+      <c r="C70" s="120" t="s">
         <v>31</v>
       </c>
       <c r="D70" s="44" t="s">
@@ -4212,10 +4233,10 @@
       <c r="R70" s="40"/>
     </row>
     <row r="71" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B71" s="125"/>
-      <c r="C71" s="126"/>
+      <c r="B71" s="121"/>
+      <c r="C71" s="120"/>
       <c r="D71" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E71" s="45"/>
       <c r="F71" s="45"/>
@@ -4236,8 +4257,8 @@
       <c r="R71" s="40"/>
     </row>
     <row r="72" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B72" s="125"/>
-      <c r="C72" s="126"/>
+      <c r="B72" s="121"/>
+      <c r="C72" s="120"/>
       <c r="D72" s="44" t="s">
         <v>35</v>
       </c>
@@ -4283,8 +4304,8 @@
       </c>
     </row>
     <row r="73" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B73" s="125"/>
-      <c r="C73" s="125"/>
+      <c r="B73" s="121"/>
+      <c r="C73" s="121"/>
       <c r="D73" s="48" t="s">
         <v>37</v>
       </c>
@@ -4330,8 +4351,8 @@
       </c>
     </row>
     <row r="74" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B74" s="125"/>
-      <c r="C74" s="125"/>
+      <c r="B74" s="121"/>
+      <c r="C74" s="121"/>
       <c r="D74" s="48" t="s">
         <v>38</v>
       </c>
@@ -4377,8 +4398,8 @@
       </c>
     </row>
     <row r="75" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B75" s="125"/>
-      <c r="C75" s="126" t="s">
+      <c r="B75" s="121"/>
+      <c r="C75" s="120" t="s">
         <v>48</v>
       </c>
       <c r="D75" s="44" t="s">
@@ -4427,8 +4448,8 @@
       <c r="R75" s="40"/>
     </row>
     <row r="76" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B76" s="125"/>
-      <c r="C76" s="125"/>
+      <c r="B76" s="121"/>
+      <c r="C76" s="121"/>
       <c r="D76" s="48" t="s">
         <v>39</v>
       </c>
@@ -4475,8 +4496,8 @@
       <c r="R76" s="40"/>
     </row>
     <row r="77" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B77" s="125"/>
-      <c r="C77" s="125"/>
+      <c r="B77" s="121"/>
+      <c r="C77" s="121"/>
       <c r="D77" s="48" t="s">
         <v>40</v>
       </c>
@@ -4523,8 +4544,8 @@
       <c r="R77" s="40"/>
     </row>
     <row r="78" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B78" s="125"/>
-      <c r="C78" s="126" t="s">
+      <c r="B78" s="121"/>
+      <c r="C78" s="120" t="s">
         <v>47</v>
       </c>
       <c r="D78" s="44" t="s">
@@ -4573,10 +4594,10 @@
       <c r="R78" s="40"/>
     </row>
     <row r="79" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B79" s="125"/>
-      <c r="C79" s="126"/>
+      <c r="B79" s="121"/>
+      <c r="C79" s="120"/>
       <c r="D79" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E79" s="46"/>
       <c r="F79" s="46"/>
@@ -4597,8 +4618,8 @@
       <c r="R79" s="40"/>
     </row>
     <row r="80" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B80" s="125"/>
-      <c r="C80" s="125"/>
+      <c r="B80" s="121"/>
+      <c r="C80" s="121"/>
       <c r="D80" s="48" t="s">
         <v>39</v>
       </c>
@@ -4645,10 +4666,10 @@
       <c r="R80" s="40"/>
     </row>
     <row r="81" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B81" s="125"/>
-      <c r="C81" s="125"/>
+      <c r="B81" s="121"/>
+      <c r="C81" s="121"/>
       <c r="D81" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E81" s="51"/>
       <c r="F81" s="51"/>
@@ -4669,8 +4690,8 @@
       <c r="R81" s="40"/>
     </row>
     <row r="82" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B82" s="125"/>
-      <c r="C82" s="125"/>
+      <c r="B82" s="121"/>
+      <c r="C82" s="121"/>
       <c r="D82" s="48" t="s">
         <v>40</v>
       </c>
@@ -4717,10 +4738,10 @@
       <c r="R82" s="40"/>
     </row>
     <row r="83" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B83" s="125" t="s">
+      <c r="B83" s="121" t="s">
         <v>33</v>
       </c>
-      <c r="C83" s="126" t="s">
+      <c r="C83" s="120" t="s">
         <v>31</v>
       </c>
       <c r="D83" s="44" t="s">
@@ -4769,8 +4790,8 @@
       <c r="R83" s="40"/>
     </row>
     <row r="84" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B84" s="125"/>
-      <c r="C84" s="126"/>
+      <c r="B84" s="121"/>
+      <c r="C84" s="120"/>
       <c r="D84" s="44" t="s">
         <v>35</v>
       </c>
@@ -4817,8 +4838,8 @@
       <c r="R84" s="40"/>
     </row>
     <row r="85" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B85" s="125"/>
-      <c r="C85" s="125"/>
+      <c r="B85" s="121"/>
+      <c r="C85" s="121"/>
       <c r="D85" s="48" t="s">
         <v>37</v>
       </c>
@@ -4865,8 +4886,8 @@
       <c r="R85" s="40"/>
     </row>
     <row r="86" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B86" s="125"/>
-      <c r="C86" s="125"/>
+      <c r="B86" s="121"/>
+      <c r="C86" s="121"/>
       <c r="D86" s="48" t="s">
         <v>38</v>
       </c>
@@ -4912,8 +4933,8 @@
       </c>
     </row>
     <row r="87" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B87" s="125"/>
-      <c r="C87" s="126" t="s">
+      <c r="B87" s="121"/>
+      <c r="C87" s="120" t="s">
         <v>48</v>
       </c>
       <c r="D87" s="44" t="s">
@@ -4961,10 +4982,10 @@
       </c>
     </row>
     <row r="88" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B88" s="125"/>
-      <c r="C88" s="126"/>
+      <c r="B88" s="121"/>
+      <c r="C88" s="120"/>
       <c r="D88" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E88" s="45"/>
       <c r="F88" s="45"/>
@@ -4984,8 +5005,8 @@
       </c>
     </row>
     <row r="89" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B89" s="125"/>
-      <c r="C89" s="125"/>
+      <c r="B89" s="121"/>
+      <c r="C89" s="121"/>
       <c r="D89" s="48" t="s">
         <v>39</v>
       </c>
@@ -5031,10 +5052,10 @@
       </c>
     </row>
     <row r="90" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B90" s="125"/>
-      <c r="C90" s="125"/>
+      <c r="B90" s="121"/>
+      <c r="C90" s="121"/>
       <c r="D90" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E90" s="53"/>
       <c r="F90" s="53"/>
@@ -5054,8 +5075,8 @@
       </c>
     </row>
     <row r="91" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B91" s="125"/>
-      <c r="C91" s="125"/>
+      <c r="B91" s="121"/>
+      <c r="C91" s="121"/>
       <c r="D91" s="48" t="s">
         <v>40</v>
       </c>
@@ -5101,8 +5122,8 @@
       </c>
     </row>
     <row r="92" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B92" s="125"/>
-      <c r="C92" s="126" t="s">
+      <c r="B92" s="121"/>
+      <c r="C92" s="120" t="s">
         <v>47</v>
       </c>
       <c r="D92" s="44" t="s">
@@ -5150,10 +5171,10 @@
       </c>
     </row>
     <row r="93" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B93" s="125"/>
-      <c r="C93" s="126"/>
+      <c r="B93" s="121"/>
+      <c r="C93" s="120"/>
       <c r="D93" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E93" s="46"/>
       <c r="F93" s="46"/>
@@ -5173,8 +5194,8 @@
       </c>
     </row>
     <row r="94" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B94" s="125"/>
-      <c r="C94" s="125"/>
+      <c r="B94" s="121"/>
+      <c r="C94" s="121"/>
       <c r="D94" s="48" t="s">
         <v>39</v>
       </c>
@@ -5220,10 +5241,10 @@
       </c>
     </row>
     <row r="95" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B95" s="125"/>
-      <c r="C95" s="125"/>
+      <c r="B95" s="121"/>
+      <c r="C95" s="121"/>
       <c r="D95" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E95" s="52"/>
       <c r="F95" s="52"/>
@@ -5243,8 +5264,8 @@
       </c>
     </row>
     <row r="96" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B96" s="125"/>
-      <c r="C96" s="125"/>
+      <c r="B96" s="121"/>
+      <c r="C96" s="121"/>
       <c r="D96" s="48" t="s">
         <v>40</v>
       </c>
@@ -5290,10 +5311,10 @@
       </c>
     </row>
     <row r="97" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B97" s="125" t="s">
+      <c r="B97" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="C97" s="126" t="s">
+      <c r="C97" s="120" t="s">
         <v>31</v>
       </c>
       <c r="D97" s="44" t="s">
@@ -5341,10 +5362,10 @@
       </c>
     </row>
     <row r="98" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B98" s="125"/>
-      <c r="C98" s="126"/>
+      <c r="B98" s="121"/>
+      <c r="C98" s="120"/>
       <c r="D98" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E98" s="45"/>
       <c r="F98" s="45"/>
@@ -5364,8 +5385,8 @@
       </c>
     </row>
     <row r="99" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B99" s="125"/>
-      <c r="C99" s="126"/>
+      <c r="B99" s="121"/>
+      <c r="C99" s="120"/>
       <c r="D99" s="44" t="s">
         <v>35</v>
       </c>
@@ -5411,8 +5432,8 @@
       </c>
     </row>
     <row r="100" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B100" s="125"/>
-      <c r="C100" s="125"/>
+      <c r="B100" s="121"/>
+      <c r="C100" s="121"/>
       <c r="D100" s="48" t="s">
         <v>37</v>
       </c>
@@ -5458,8 +5479,8 @@
       </c>
     </row>
     <row r="101" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B101" s="125"/>
-      <c r="C101" s="125"/>
+      <c r="B101" s="121"/>
+      <c r="C101" s="121"/>
       <c r="D101" s="48" t="s">
         <v>38</v>
       </c>
@@ -5505,8 +5526,8 @@
       </c>
     </row>
     <row r="102" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B102" s="125"/>
-      <c r="C102" s="126" t="s">
+      <c r="B102" s="121"/>
+      <c r="C102" s="120" t="s">
         <v>48</v>
       </c>
       <c r="D102" s="44" t="s">
@@ -5554,10 +5575,10 @@
       </c>
     </row>
     <row r="103" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B103" s="125"/>
-      <c r="C103" s="126"/>
+      <c r="B103" s="121"/>
+      <c r="C103" s="120"/>
       <c r="D103" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E103" s="45"/>
       <c r="F103" s="45"/>
@@ -5577,8 +5598,8 @@
       </c>
     </row>
     <row r="104" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B104" s="125"/>
-      <c r="C104" s="125"/>
+      <c r="B104" s="121"/>
+      <c r="C104" s="121"/>
       <c r="D104" s="48" t="s">
         <v>39</v>
       </c>
@@ -5624,10 +5645,10 @@
       </c>
     </row>
     <row r="105" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B105" s="125"/>
-      <c r="C105" s="125"/>
+      <c r="B105" s="121"/>
+      <c r="C105" s="121"/>
       <c r="D105" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E105" s="50"/>
       <c r="F105" s="50"/>
@@ -5647,8 +5668,8 @@
       </c>
     </row>
     <row r="106" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B106" s="125"/>
-      <c r="C106" s="125"/>
+      <c r="B106" s="121"/>
+      <c r="C106" s="121"/>
       <c r="D106" s="48" t="s">
         <v>40</v>
       </c>
@@ -5694,8 +5715,8 @@
       </c>
     </row>
     <row r="107" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B107" s="125"/>
-      <c r="C107" s="126" t="s">
+      <c r="B107" s="121"/>
+      <c r="C107" s="120" t="s">
         <v>47</v>
       </c>
       <c r="D107" s="44" t="s">
@@ -5743,10 +5764,10 @@
       </c>
     </row>
     <row r="108" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B108" s="125"/>
-      <c r="C108" s="126"/>
+      <c r="B108" s="121"/>
+      <c r="C108" s="120"/>
       <c r="D108" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E108" s="46"/>
       <c r="F108" s="46"/>
@@ -5766,8 +5787,8 @@
       </c>
     </row>
     <row r="109" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B109" s="125"/>
-      <c r="C109" s="125"/>
+      <c r="B109" s="121"/>
+      <c r="C109" s="121"/>
       <c r="D109" s="48" t="s">
         <v>39</v>
       </c>
@@ -5814,10 +5835,10 @@
     </row>
     <row r="110" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="23"/>
-      <c r="B110" s="125"/>
-      <c r="C110" s="125"/>
+      <c r="B110" s="121"/>
+      <c r="C110" s="121"/>
       <c r="D110" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E110" s="51"/>
       <c r="F110" s="51"/>
@@ -5838,8 +5859,8 @@
       <c r="O110" s="23"/>
     </row>
     <row r="111" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B111" s="125"/>
-      <c r="C111" s="125"/>
+      <c r="B111" s="121"/>
+      <c r="C111" s="121"/>
       <c r="D111" s="48" t="s">
         <v>40</v>
       </c>
@@ -5900,7 +5921,7 @@
       <c r="N112" s="68"/>
     </row>
     <row r="113" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B113" s="127" t="s">
+      <c r="B113" s="122" t="s">
         <v>20</v>
       </c>
       <c r="C113" s="85" t="s">
@@ -5910,39 +5931,39 @@
         <f>E9</f>
         <v>0.2</v>
       </c>
-      <c r="E113" s="117" t="s">
+      <c r="E113" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="F113" s="117" t="s">
+      <c r="F113" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="G113" s="117" t="s">
+      <c r="G113" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="H113" s="117" t="s">
+      <c r="H113" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="I113" s="117" t="s">
+      <c r="I113" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="J113" s="117" t="s">
+      <c r="J113" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="K113" s="117" t="s">
+      <c r="K113" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="L113" s="117" t="s">
+      <c r="L113" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="M113" s="117" t="s">
+      <c r="M113" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="N113" s="117" t="s">
+      <c r="N113" s="118" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="114" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B114" s="128"/>
+      <c r="B114" s="123"/>
       <c r="C114" s="87" t="s">
         <v>50</v>
       </c>
@@ -5950,22 +5971,22 @@
         <f>"10 BTC / "&amp;TEXT($E$4*10, "$###0.00,,")&amp;"M USD"</f>
         <v>10 BTC / $1.00M USD</v>
       </c>
-      <c r="E114" s="118"/>
-      <c r="F114" s="118"/>
-      <c r="G114" s="118"/>
-      <c r="H114" s="118"/>
-      <c r="I114" s="118"/>
-      <c r="J114" s="118"/>
-      <c r="K114" s="118"/>
-      <c r="L114" s="118"/>
-      <c r="M114" s="118"/>
-      <c r="N114" s="118"/>
+      <c r="E114" s="119"/>
+      <c r="F114" s="119"/>
+      <c r="G114" s="119"/>
+      <c r="H114" s="119"/>
+      <c r="I114" s="119"/>
+      <c r="J114" s="119"/>
+      <c r="K114" s="119"/>
+      <c r="L114" s="119"/>
+      <c r="M114" s="119"/>
+      <c r="N114" s="119"/>
     </row>
     <row r="115" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B115" s="125" t="s">
+      <c r="B115" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="C115" s="126" t="s">
+      <c r="C115" s="120" t="s">
         <v>31</v>
       </c>
       <c r="D115" s="44" t="s">
@@ -6013,10 +6034,10 @@
       </c>
     </row>
     <row r="116" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B116" s="125"/>
-      <c r="C116" s="126"/>
+      <c r="B116" s="121"/>
+      <c r="C116" s="120"/>
       <c r="D116" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E116" s="45"/>
       <c r="F116" s="45"/>
@@ -6036,8 +6057,8 @@
       </c>
     </row>
     <row r="117" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B117" s="125"/>
-      <c r="C117" s="126"/>
+      <c r="B117" s="121"/>
+      <c r="C117" s="120"/>
       <c r="D117" s="44" t="s">
         <v>35</v>
       </c>
@@ -6083,8 +6104,8 @@
       </c>
     </row>
     <row r="118" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B118" s="125"/>
-      <c r="C118" s="125"/>
+      <c r="B118" s="121"/>
+      <c r="C118" s="121"/>
       <c r="D118" s="48" t="s">
         <v>37</v>
       </c>
@@ -6130,8 +6151,8 @@
       </c>
     </row>
     <row r="119" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B119" s="125"/>
-      <c r="C119" s="125"/>
+      <c r="B119" s="121"/>
+      <c r="C119" s="121"/>
       <c r="D119" s="48" t="s">
         <v>38</v>
       </c>
@@ -6177,8 +6198,8 @@
       </c>
     </row>
     <row r="120" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B120" s="125"/>
-      <c r="C120" s="126" t="s">
+      <c r="B120" s="121"/>
+      <c r="C120" s="120" t="s">
         <v>48</v>
       </c>
       <c r="D120" s="44" t="s">
@@ -6226,8 +6247,8 @@
       </c>
     </row>
     <row r="121" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B121" s="125"/>
-      <c r="C121" s="125"/>
+      <c r="B121" s="121"/>
+      <c r="C121" s="121"/>
       <c r="D121" s="48" t="s">
         <v>39</v>
       </c>
@@ -6273,8 +6294,8 @@
       </c>
     </row>
     <row r="122" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B122" s="125"/>
-      <c r="C122" s="125"/>
+      <c r="B122" s="121"/>
+      <c r="C122" s="121"/>
       <c r="D122" s="48" t="s">
         <v>40</v>
       </c>
@@ -6320,8 +6341,8 @@
       </c>
     </row>
     <row r="123" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B123" s="125"/>
-      <c r="C123" s="126" t="s">
+      <c r="B123" s="121"/>
+      <c r="C123" s="120" t="s">
         <v>47</v>
       </c>
       <c r="D123" s="44" t="s">
@@ -6369,10 +6390,10 @@
       </c>
     </row>
     <row r="124" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B124" s="125"/>
-      <c r="C124" s="126"/>
+      <c r="B124" s="121"/>
+      <c r="C124" s="120"/>
       <c r="D124" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E124" s="46"/>
       <c r="F124" s="46"/>
@@ -6392,8 +6413,8 @@
       </c>
     </row>
     <row r="125" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B125" s="125"/>
-      <c r="C125" s="125"/>
+      <c r="B125" s="121"/>
+      <c r="C125" s="121"/>
       <c r="D125" s="48" t="s">
         <v>39</v>
       </c>
@@ -6439,10 +6460,10 @@
       </c>
     </row>
     <row r="126" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B126" s="125"/>
-      <c r="C126" s="125"/>
+      <c r="B126" s="121"/>
+      <c r="C126" s="121"/>
       <c r="D126" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E126" s="51"/>
       <c r="F126" s="51"/>
@@ -6462,8 +6483,8 @@
       </c>
     </row>
     <row r="127" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B127" s="125"/>
-      <c r="C127" s="125"/>
+      <c r="B127" s="121"/>
+      <c r="C127" s="121"/>
       <c r="D127" s="48" t="s">
         <v>40</v>
       </c>
@@ -6509,10 +6530,10 @@
       </c>
     </row>
     <row r="128" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B128" s="125" t="s">
+      <c r="B128" s="121" t="s">
         <v>33</v>
       </c>
-      <c r="C128" s="126" t="s">
+      <c r="C128" s="120" t="s">
         <v>31</v>
       </c>
       <c r="D128" s="44" t="s">
@@ -6560,8 +6581,8 @@
       </c>
     </row>
     <row r="129" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B129" s="125"/>
-      <c r="C129" s="126"/>
+      <c r="B129" s="121"/>
+      <c r="C129" s="120"/>
       <c r="D129" s="44" t="s">
         <v>35</v>
       </c>
@@ -6607,8 +6628,8 @@
       </c>
     </row>
     <row r="130" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B130" s="125"/>
-      <c r="C130" s="125"/>
+      <c r="B130" s="121"/>
+      <c r="C130" s="121"/>
       <c r="D130" s="48" t="s">
         <v>37</v>
       </c>
@@ -6654,8 +6675,8 @@
       </c>
     </row>
     <row r="131" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B131" s="125"/>
-      <c r="C131" s="125"/>
+      <c r="B131" s="121"/>
+      <c r="C131" s="121"/>
       <c r="D131" s="48" t="s">
         <v>38</v>
       </c>
@@ -6701,8 +6722,8 @@
       </c>
     </row>
     <row r="132" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B132" s="125"/>
-      <c r="C132" s="126" t="s">
+      <c r="B132" s="121"/>
+      <c r="C132" s="120" t="s">
         <v>48</v>
       </c>
       <c r="D132" s="44" t="s">
@@ -6750,10 +6771,10 @@
       </c>
     </row>
     <row r="133" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B133" s="125"/>
-      <c r="C133" s="126"/>
+      <c r="B133" s="121"/>
+      <c r="C133" s="120"/>
       <c r="D133" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E133" s="45"/>
       <c r="F133" s="45"/>
@@ -6773,8 +6794,8 @@
       </c>
     </row>
     <row r="134" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B134" s="125"/>
-      <c r="C134" s="125"/>
+      <c r="B134" s="121"/>
+      <c r="C134" s="121"/>
       <c r="D134" s="48" t="s">
         <v>39</v>
       </c>
@@ -6820,10 +6841,10 @@
       </c>
     </row>
     <row r="135" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B135" s="125"/>
-      <c r="C135" s="125"/>
+      <c r="B135" s="121"/>
+      <c r="C135" s="121"/>
       <c r="D135" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E135" s="53"/>
       <c r="F135" s="53"/>
@@ -6843,8 +6864,8 @@
       </c>
     </row>
     <row r="136" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B136" s="125"/>
-      <c r="C136" s="125"/>
+      <c r="B136" s="121"/>
+      <c r="C136" s="121"/>
       <c r="D136" s="48" t="s">
         <v>40</v>
       </c>
@@ -6890,8 +6911,8 @@
       </c>
     </row>
     <row r="137" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B137" s="125"/>
-      <c r="C137" s="126" t="s">
+      <c r="B137" s="121"/>
+      <c r="C137" s="120" t="s">
         <v>47</v>
       </c>
       <c r="D137" s="44" t="s">
@@ -6939,10 +6960,10 @@
       </c>
     </row>
     <row r="138" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B138" s="125"/>
-      <c r="C138" s="126"/>
+      <c r="B138" s="121"/>
+      <c r="C138" s="120"/>
       <c r="D138" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E138" s="46"/>
       <c r="F138" s="46"/>
@@ -6962,8 +6983,8 @@
       </c>
     </row>
     <row r="139" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B139" s="125"/>
-      <c r="C139" s="125"/>
+      <c r="B139" s="121"/>
+      <c r="C139" s="121"/>
       <c r="D139" s="48" t="s">
         <v>39</v>
       </c>
@@ -7009,10 +7030,10 @@
       </c>
     </row>
     <row r="140" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B140" s="125"/>
-      <c r="C140" s="125"/>
+      <c r="B140" s="121"/>
+      <c r="C140" s="121"/>
       <c r="D140" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E140" s="52"/>
       <c r="F140" s="52"/>
@@ -7032,8 +7053,8 @@
       </c>
     </row>
     <row r="141" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B141" s="125"/>
-      <c r="C141" s="125"/>
+      <c r="B141" s="121"/>
+      <c r="C141" s="121"/>
       <c r="D141" s="48" t="s">
         <v>40</v>
       </c>
@@ -7079,10 +7100,10 @@
       </c>
     </row>
     <row r="142" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B142" s="125" t="s">
+      <c r="B142" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="C142" s="126" t="s">
+      <c r="C142" s="120" t="s">
         <v>31</v>
       </c>
       <c r="D142" s="44" t="s">
@@ -7130,10 +7151,10 @@
       </c>
     </row>
     <row r="143" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B143" s="125"/>
-      <c r="C143" s="126"/>
+      <c r="B143" s="121"/>
+      <c r="C143" s="120"/>
       <c r="D143" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E143" s="45"/>
       <c r="F143" s="45"/>
@@ -7153,8 +7174,8 @@
       </c>
     </row>
     <row r="144" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B144" s="125"/>
-      <c r="C144" s="126"/>
+      <c r="B144" s="121"/>
+      <c r="C144" s="120"/>
       <c r="D144" s="44" t="s">
         <v>35</v>
       </c>
@@ -7200,8 +7221,8 @@
       </c>
     </row>
     <row r="145" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B145" s="125"/>
-      <c r="C145" s="125"/>
+      <c r="B145" s="121"/>
+      <c r="C145" s="121"/>
       <c r="D145" s="48" t="s">
         <v>37</v>
       </c>
@@ -7247,8 +7268,8 @@
       </c>
     </row>
     <row r="146" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B146" s="125"/>
-      <c r="C146" s="125"/>
+      <c r="B146" s="121"/>
+      <c r="C146" s="121"/>
       <c r="D146" s="48" t="s">
         <v>38</v>
       </c>
@@ -7294,8 +7315,8 @@
       </c>
     </row>
     <row r="147" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B147" s="125"/>
-      <c r="C147" s="126" t="s">
+      <c r="B147" s="121"/>
+      <c r="C147" s="120" t="s">
         <v>48</v>
       </c>
       <c r="D147" s="44" t="s">
@@ -7343,10 +7364,10 @@
       </c>
     </row>
     <row r="148" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B148" s="125"/>
-      <c r="C148" s="126"/>
+      <c r="B148" s="121"/>
+      <c r="C148" s="120"/>
       <c r="D148" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E148" s="45"/>
       <c r="F148" s="45"/>
@@ -7366,8 +7387,8 @@
       </c>
     </row>
     <row r="149" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B149" s="125"/>
-      <c r="C149" s="125"/>
+      <c r="B149" s="121"/>
+      <c r="C149" s="121"/>
       <c r="D149" s="48" t="s">
         <v>39</v>
       </c>
@@ -7413,10 +7434,10 @@
       </c>
     </row>
     <row r="150" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B150" s="125"/>
-      <c r="C150" s="125"/>
+      <c r="B150" s="121"/>
+      <c r="C150" s="121"/>
       <c r="D150" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E150" s="50"/>
       <c r="F150" s="50"/>
@@ -7436,8 +7457,8 @@
       </c>
     </row>
     <row r="151" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B151" s="125"/>
-      <c r="C151" s="125"/>
+      <c r="B151" s="121"/>
+      <c r="C151" s="121"/>
       <c r="D151" s="48" t="s">
         <v>40</v>
       </c>
@@ -7483,8 +7504,8 @@
       </c>
     </row>
     <row r="152" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B152" s="125"/>
-      <c r="C152" s="126" t="s">
+      <c r="B152" s="121"/>
+      <c r="C152" s="120" t="s">
         <v>47</v>
       </c>
       <c r="D152" s="44" t="s">
@@ -7533,10 +7554,10 @@
     </row>
     <row r="153" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153" s="23"/>
-      <c r="B153" s="125"/>
-      <c r="C153" s="126"/>
+      <c r="B153" s="121"/>
+      <c r="C153" s="120"/>
       <c r="D153" s="44" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E153" s="46"/>
       <c r="F153" s="46"/>
@@ -7557,8 +7578,8 @@
       <c r="O153" s="23"/>
     </row>
     <row r="154" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B154" s="125"/>
-      <c r="C154" s="125"/>
+      <c r="B154" s="121"/>
+      <c r="C154" s="121"/>
       <c r="D154" s="48" t="s">
         <v>39</v>
       </c>
@@ -7604,10 +7625,10 @@
       </c>
     </row>
     <row r="155" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B155" s="125"/>
-      <c r="C155" s="125"/>
+      <c r="B155" s="121"/>
+      <c r="C155" s="121"/>
       <c r="D155" s="48" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E155" s="51"/>
       <c r="F155" s="51"/>
@@ -7627,8 +7648,8 @@
       </c>
     </row>
     <row r="156" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B156" s="125"/>
-      <c r="C156" s="125"/>
+      <c r="B156" s="121"/>
+      <c r="C156" s="121"/>
       <c r="D156" s="48" t="s">
         <v>40</v>
       </c>
@@ -7689,62 +7710,62 @@
       <c r="N157" s="29"/>
     </row>
     <row r="158" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B158" s="119" t="s">
+      <c r="B158" s="139" t="s">
         <v>53</v>
       </c>
       <c r="C158" s="89"/>
       <c r="D158" s="90"/>
-      <c r="E158" s="117" t="s">
+      <c r="E158" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="F158" s="117" t="s">
+      <c r="F158" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="G158" s="117" t="s">
+      <c r="G158" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="H158" s="117" t="s">
+      <c r="H158" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="I158" s="117" t="s">
+      <c r="I158" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="J158" s="117" t="s">
+      <c r="J158" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="K158" s="117" t="s">
+      <c r="K158" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="L158" s="117" t="s">
+      <c r="L158" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="M158" s="117" t="s">
+      <c r="M158" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="N158" s="117" t="s">
+      <c r="N158" s="118" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="159" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B159" s="120"/>
+      <c r="B159" s="140"/>
       <c r="C159" s="65"/>
       <c r="D159" s="66"/>
-      <c r="E159" s="118"/>
-      <c r="F159" s="118"/>
-      <c r="G159" s="118"/>
-      <c r="H159" s="118"/>
-      <c r="I159" s="118"/>
-      <c r="J159" s="118"/>
-      <c r="K159" s="118"/>
-      <c r="L159" s="118"/>
-      <c r="M159" s="118"/>
-      <c r="N159" s="118"/>
+      <c r="E159" s="119"/>
+      <c r="F159" s="119"/>
+      <c r="G159" s="119"/>
+      <c r="H159" s="119"/>
+      <c r="I159" s="119"/>
+      <c r="J159" s="119"/>
+      <c r="K159" s="119"/>
+      <c r="L159" s="119"/>
+      <c r="M159" s="119"/>
+      <c r="N159" s="119"/>
     </row>
     <row r="160" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B160" s="125" t="s">
+      <c r="B160" s="121" t="s">
         <v>32</v>
       </c>
-      <c r="C160" s="123">
+      <c r="C160" s="124">
         <v>20000</v>
       </c>
       <c r="D160" s="48" t="s">
@@ -7792,10 +7813,10 @@
       </c>
     </row>
     <row r="161" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B161" s="125"/>
-      <c r="C161" s="123"/>
+      <c r="B161" s="121"/>
+      <c r="C161" s="124"/>
       <c r="D161" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E161" s="57"/>
       <c r="F161" s="57"/>
@@ -7815,10 +7836,10 @@
       </c>
     </row>
     <row r="162" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B162" s="125"/>
-      <c r="C162" s="123"/>
+      <c r="B162" s="121"/>
+      <c r="C162" s="124"/>
       <c r="D162" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E162" s="57">
         <f>E$119*$C160/20</f>
@@ -7862,8 +7883,8 @@
       </c>
     </row>
     <row r="163" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B163" s="125"/>
-      <c r="C163" s="123">
+      <c r="B163" s="121"/>
+      <c r="C163" s="124">
         <v>400000</v>
       </c>
       <c r="D163" s="48" t="s">
@@ -7911,10 +7932,10 @@
       </c>
     </row>
     <row r="164" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B164" s="125"/>
-      <c r="C164" s="123"/>
+      <c r="B164" s="121"/>
+      <c r="C164" s="124"/>
       <c r="D164" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E164" s="57"/>
       <c r="F164" s="57"/>
@@ -7934,10 +7955,10 @@
       </c>
     </row>
     <row r="165" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B165" s="125"/>
-      <c r="C165" s="123"/>
+      <c r="B165" s="121"/>
+      <c r="C165" s="124"/>
       <c r="D165" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E165" s="57">
         <f>E$119*$C163/20</f>
@@ -7981,8 +8002,8 @@
       </c>
     </row>
     <row r="166" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B166" s="126"/>
-      <c r="C166" s="124">
+      <c r="B166" s="120"/>
+      <c r="C166" s="125">
         <v>1000000</v>
       </c>
       <c r="D166" s="44" t="s">
@@ -8030,10 +8051,10 @@
       </c>
     </row>
     <row r="167" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B167" s="126"/>
-      <c r="C167" s="124"/>
+      <c r="B167" s="120"/>
+      <c r="C167" s="125"/>
       <c r="D167" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E167" s="59"/>
       <c r="F167" s="59"/>
@@ -8053,10 +8074,10 @@
       </c>
     </row>
     <row r="168" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B168" s="126"/>
-      <c r="C168" s="124"/>
+      <c r="B168" s="120"/>
+      <c r="C168" s="125"/>
       <c r="D168" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E168" s="59">
         <f>E$119*$C166/20</f>
@@ -8100,8 +8121,8 @@
       </c>
     </row>
     <row r="169" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B169" s="126"/>
-      <c r="C169" s="124">
+      <c r="B169" s="120"/>
+      <c r="C169" s="125">
         <v>2100000</v>
       </c>
       <c r="D169" s="44" t="s">
@@ -8149,10 +8170,10 @@
       </c>
     </row>
     <row r="170" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B170" s="126"/>
-      <c r="C170" s="124"/>
+      <c r="B170" s="120"/>
+      <c r="C170" s="125"/>
       <c r="D170" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E170" s="59"/>
       <c r="F170" s="59"/>
@@ -8172,10 +8193,10 @@
       </c>
     </row>
     <row r="171" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B171" s="126"/>
-      <c r="C171" s="124"/>
+      <c r="B171" s="120"/>
+      <c r="C171" s="125"/>
       <c r="D171" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E171" s="59">
         <f>E$119*$C169/20</f>
@@ -8219,10 +8240,10 @@
       </c>
     </row>
     <row r="172" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B172" s="125" t="s">
+      <c r="B172" s="121" t="s">
         <v>33</v>
       </c>
-      <c r="C172" s="123">
+      <c r="C172" s="124">
         <v>20000</v>
       </c>
       <c r="D172" s="48" t="s">
@@ -8270,10 +8291,10 @@
       </c>
     </row>
     <row r="173" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B173" s="125"/>
-      <c r="C173" s="123"/>
+      <c r="B173" s="121"/>
+      <c r="C173" s="124"/>
       <c r="D173" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E173" s="57"/>
       <c r="F173" s="57"/>
@@ -8293,10 +8314,10 @@
       </c>
     </row>
     <row r="174" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B174" s="125"/>
-      <c r="C174" s="123"/>
+      <c r="B174" s="121"/>
+      <c r="C174" s="124"/>
       <c r="D174" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E174" s="57">
         <f>E$129*$C172/20</f>
@@ -8340,8 +8361,8 @@
       </c>
     </row>
     <row r="175" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B175" s="125"/>
-      <c r="C175" s="123">
+      <c r="B175" s="121"/>
+      <c r="C175" s="124">
         <v>400000</v>
       </c>
       <c r="D175" s="48" t="s">
@@ -8389,10 +8410,10 @@
       </c>
     </row>
     <row r="176" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B176" s="125"/>
-      <c r="C176" s="123"/>
+      <c r="B176" s="121"/>
+      <c r="C176" s="124"/>
       <c r="D176" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E176" s="57"/>
       <c r="F176" s="57"/>
@@ -8412,10 +8433,10 @@
       </c>
     </row>
     <row r="177" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B177" s="125"/>
-      <c r="C177" s="123"/>
+      <c r="B177" s="121"/>
+      <c r="C177" s="124"/>
       <c r="D177" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E177" s="57">
         <f>E$129*$C175/20</f>
@@ -8459,8 +8480,8 @@
       </c>
     </row>
     <row r="178" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B178" s="125"/>
-      <c r="C178" s="124">
+      <c r="B178" s="121"/>
+      <c r="C178" s="125">
         <v>1000000</v>
       </c>
       <c r="D178" s="44" t="s">
@@ -8508,10 +8529,10 @@
       </c>
     </row>
     <row r="179" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B179" s="125"/>
-      <c r="C179" s="124"/>
+      <c r="B179" s="121"/>
+      <c r="C179" s="125"/>
       <c r="D179" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E179" s="59"/>
       <c r="F179" s="59"/>
@@ -8531,10 +8552,10 @@
       </c>
     </row>
     <row r="180" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B180" s="125"/>
-      <c r="C180" s="124"/>
+      <c r="B180" s="121"/>
+      <c r="C180" s="125"/>
       <c r="D180" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E180" s="59">
         <f>E$129*$C178/20</f>
@@ -8578,8 +8599,8 @@
       </c>
     </row>
     <row r="181" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B181" s="125"/>
-      <c r="C181" s="124">
+      <c r="B181" s="121"/>
+      <c r="C181" s="125">
         <v>2100000</v>
       </c>
       <c r="D181" s="44" t="s">
@@ -8627,10 +8648,10 @@
       </c>
     </row>
     <row r="182" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B182" s="125"/>
-      <c r="C182" s="124"/>
+      <c r="B182" s="121"/>
+      <c r="C182" s="125"/>
       <c r="D182" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E182" s="59"/>
       <c r="F182" s="59"/>
@@ -8650,10 +8671,10 @@
       </c>
     </row>
     <row r="183" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B183" s="125"/>
-      <c r="C183" s="124"/>
+      <c r="B183" s="121"/>
+      <c r="C183" s="125"/>
       <c r="D183" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E183" s="59">
         <f>E$129*$C181/20</f>
@@ -8697,10 +8718,10 @@
       </c>
     </row>
     <row r="184" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B184" s="125" t="s">
+      <c r="B184" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="C184" s="123">
+      <c r="C184" s="124">
         <v>20000</v>
       </c>
       <c r="D184" s="48" t="s">
@@ -8748,10 +8769,10 @@
       </c>
     </row>
     <row r="185" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B185" s="125"/>
-      <c r="C185" s="123"/>
+      <c r="B185" s="121"/>
+      <c r="C185" s="124"/>
       <c r="D185" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E185" s="57"/>
       <c r="F185" s="57"/>
@@ -8771,10 +8792,10 @@
       </c>
     </row>
     <row r="186" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B186" s="125"/>
-      <c r="C186" s="123"/>
+      <c r="B186" s="121"/>
+      <c r="C186" s="124"/>
       <c r="D186" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E186" s="57">
         <f>E162+E174</f>
@@ -8818,8 +8839,8 @@
       </c>
     </row>
     <row r="187" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B187" s="125"/>
-      <c r="C187" s="123">
+      <c r="B187" s="121"/>
+      <c r="C187" s="124">
         <v>400000</v>
       </c>
       <c r="D187" s="48" t="s">
@@ -8867,10 +8888,10 @@
       </c>
     </row>
     <row r="188" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B188" s="125"/>
-      <c r="C188" s="123"/>
+      <c r="B188" s="121"/>
+      <c r="C188" s="124"/>
       <c r="D188" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E188" s="57"/>
       <c r="F188" s="57"/>
@@ -8890,10 +8911,10 @@
       </c>
     </row>
     <row r="189" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B189" s="125"/>
-      <c r="C189" s="123"/>
+      <c r="B189" s="121"/>
+      <c r="C189" s="124"/>
       <c r="D189" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E189" s="57">
         <f>E165+E177</f>
@@ -8937,8 +8958,8 @@
       </c>
     </row>
     <row r="190" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B190" s="125"/>
-      <c r="C190" s="124">
+      <c r="B190" s="121"/>
+      <c r="C190" s="125">
         <v>1000000</v>
       </c>
       <c r="D190" s="44" t="s">
@@ -8986,10 +9007,10 @@
       </c>
     </row>
     <row r="191" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B191" s="125"/>
-      <c r="C191" s="124"/>
+      <c r="B191" s="121"/>
+      <c r="C191" s="125"/>
       <c r="D191" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E191" s="59"/>
       <c r="F191" s="59"/>
@@ -9009,10 +9030,10 @@
       </c>
     </row>
     <row r="192" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B192" s="125"/>
-      <c r="C192" s="124"/>
+      <c r="B192" s="121"/>
+      <c r="C192" s="125"/>
       <c r="D192" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E192" s="59">
         <f>E168+E180</f>
@@ -9056,8 +9077,8 @@
       </c>
     </row>
     <row r="193" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B193" s="125"/>
-      <c r="C193" s="124">
+      <c r="B193" s="121"/>
+      <c r="C193" s="125">
         <v>2100000</v>
       </c>
       <c r="D193" s="44" t="s">
@@ -9105,10 +9126,10 @@
       </c>
     </row>
     <row r="194" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B194" s="125"/>
-      <c r="C194" s="124"/>
+      <c r="B194" s="121"/>
+      <c r="C194" s="125"/>
       <c r="D194" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E194" s="59"/>
       <c r="F194" s="59"/>
@@ -9128,10 +9149,10 @@
       </c>
     </row>
     <row r="195" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B195" s="125"/>
-      <c r="C195" s="124"/>
+      <c r="B195" s="121"/>
+      <c r="C195" s="125"/>
       <c r="D195" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E195" s="59">
         <f>E171+E183</f>
@@ -9203,95 +9224,8 @@
       <c r="N197" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="112">
-    <mergeCell ref="B20:C21"/>
-    <mergeCell ref="B16:C19"/>
-    <mergeCell ref="B14:C15"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="B70:B82"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="C47:C51"/>
-    <mergeCell ref="B38:B51"/>
-    <mergeCell ref="C57:C61"/>
-    <mergeCell ref="C62:C66"/>
-    <mergeCell ref="B52:B66"/>
-    <mergeCell ref="C70:C74"/>
-    <mergeCell ref="C75:C77"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="B83:B96"/>
-    <mergeCell ref="B97:B111"/>
-    <mergeCell ref="B115:B127"/>
-    <mergeCell ref="C115:C119"/>
-    <mergeCell ref="C120:C122"/>
-    <mergeCell ref="C123:C127"/>
-    <mergeCell ref="C83:C86"/>
-    <mergeCell ref="C87:C91"/>
-    <mergeCell ref="C92:C96"/>
-    <mergeCell ref="C97:C101"/>
-    <mergeCell ref="C102:C106"/>
-    <mergeCell ref="C107:C111"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="B184:B195"/>
-    <mergeCell ref="C184:C186"/>
-    <mergeCell ref="C187:C189"/>
-    <mergeCell ref="C190:C192"/>
-    <mergeCell ref="C193:C195"/>
-    <mergeCell ref="C137:C141"/>
-    <mergeCell ref="B142:B156"/>
-    <mergeCell ref="C142:C146"/>
-    <mergeCell ref="C147:C151"/>
-    <mergeCell ref="C152:C156"/>
-    <mergeCell ref="B128:B141"/>
-    <mergeCell ref="C128:C131"/>
-    <mergeCell ref="C132:C136"/>
-    <mergeCell ref="C160:C162"/>
-    <mergeCell ref="C163:C165"/>
-    <mergeCell ref="C166:C168"/>
-    <mergeCell ref="C169:C171"/>
-    <mergeCell ref="B160:B171"/>
-    <mergeCell ref="B172:B183"/>
-    <mergeCell ref="C172:C174"/>
-    <mergeCell ref="C175:C177"/>
-    <mergeCell ref="C178:C180"/>
-    <mergeCell ref="C181:C183"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="H68:H69"/>
-    <mergeCell ref="I68:I69"/>
-    <mergeCell ref="J68:J69"/>
-    <mergeCell ref="K68:K69"/>
-    <mergeCell ref="L68:L69"/>
-    <mergeCell ref="M68:M69"/>
-    <mergeCell ref="N68:N69"/>
-    <mergeCell ref="B25:B37"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="H158:H159"/>
-    <mergeCell ref="J113:J114"/>
-    <mergeCell ref="K113:K114"/>
-    <mergeCell ref="L113:L114"/>
-    <mergeCell ref="M113:M114"/>
-    <mergeCell ref="N113:N114"/>
-    <mergeCell ref="E113:E114"/>
-    <mergeCell ref="F113:F114"/>
-    <mergeCell ref="G113:G114"/>
-    <mergeCell ref="H113:H114"/>
-    <mergeCell ref="I113:I114"/>
+  <mergeCells count="113">
+    <mergeCell ref="K2:M2"/>
     <mergeCell ref="B2:C10"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="G2:I3"/>
@@ -9316,6 +9250,94 @@
     <mergeCell ref="E158:E159"/>
     <mergeCell ref="F158:F159"/>
     <mergeCell ref="G158:G159"/>
+    <mergeCell ref="H158:H159"/>
+    <mergeCell ref="J113:J114"/>
+    <mergeCell ref="K113:K114"/>
+    <mergeCell ref="L113:L114"/>
+    <mergeCell ref="M113:M114"/>
+    <mergeCell ref="N113:N114"/>
+    <mergeCell ref="E113:E114"/>
+    <mergeCell ref="F113:F114"/>
+    <mergeCell ref="G113:G114"/>
+    <mergeCell ref="H113:H114"/>
+    <mergeCell ref="I113:I114"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="H68:H69"/>
+    <mergeCell ref="I68:I69"/>
+    <mergeCell ref="J68:J69"/>
+    <mergeCell ref="K68:K69"/>
+    <mergeCell ref="L68:L69"/>
+    <mergeCell ref="M68:M69"/>
+    <mergeCell ref="N68:N69"/>
+    <mergeCell ref="B25:B37"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="B184:B195"/>
+    <mergeCell ref="C184:C186"/>
+    <mergeCell ref="C187:C189"/>
+    <mergeCell ref="C190:C192"/>
+    <mergeCell ref="C193:C195"/>
+    <mergeCell ref="C137:C141"/>
+    <mergeCell ref="B142:B156"/>
+    <mergeCell ref="C142:C146"/>
+    <mergeCell ref="C147:C151"/>
+    <mergeCell ref="C152:C156"/>
+    <mergeCell ref="B128:B141"/>
+    <mergeCell ref="C128:C131"/>
+    <mergeCell ref="C132:C136"/>
+    <mergeCell ref="C160:C162"/>
+    <mergeCell ref="C163:C165"/>
+    <mergeCell ref="C166:C168"/>
+    <mergeCell ref="C169:C171"/>
+    <mergeCell ref="B160:B171"/>
+    <mergeCell ref="B172:B183"/>
+    <mergeCell ref="C172:C174"/>
+    <mergeCell ref="C175:C177"/>
+    <mergeCell ref="C178:C180"/>
+    <mergeCell ref="C181:C183"/>
+    <mergeCell ref="B83:B96"/>
+    <mergeCell ref="B97:B111"/>
+    <mergeCell ref="B115:B127"/>
+    <mergeCell ref="C115:C119"/>
+    <mergeCell ref="C120:C122"/>
+    <mergeCell ref="C123:C127"/>
+    <mergeCell ref="C83:C86"/>
+    <mergeCell ref="C87:C91"/>
+    <mergeCell ref="C92:C96"/>
+    <mergeCell ref="C97:C101"/>
+    <mergeCell ref="C102:C106"/>
+    <mergeCell ref="C107:C111"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="B70:B82"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="C47:C51"/>
+    <mergeCell ref="B38:B51"/>
+    <mergeCell ref="C57:C61"/>
+    <mergeCell ref="C62:C66"/>
+    <mergeCell ref="B52:B66"/>
+    <mergeCell ref="C70:C74"/>
+    <mergeCell ref="C75:C77"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="B20:C21"/>
+    <mergeCell ref="B16:C19"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
   </mergeCells>
   <conditionalFormatting sqref="E10">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
@@ -9378,16 +9400,16 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="16"/>
-      <c r="E2" s="137" t="s">
+      <c r="E2" s="141" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
-      <c r="L2" s="137"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="141"/>
+      <c r="K2" s="141"/>
+      <c r="L2" s="141"/>
       <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9399,14 +9421,14 @@
         <v>100000</v>
       </c>
       <c r="D3" s="16"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="137"/>
-      <c r="K3" s="137"/>
-      <c r="L3" s="137"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="141"/>
+      <c r="K3" s="141"/>
+      <c r="L3" s="141"/>
       <c r="M3" s="9"/>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -9426,18 +9448,18 @@
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="9"/>
-      <c r="B5" s="138" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="140" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" s="141">
+      <c r="B5" s="104" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="106" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="107">
         <f>(G6/C6)^(1/DATEDIF(E6,I6,"Y"))-1</f>
         <v>0.76925197017405411</v>
       </c>
@@ -9448,28 +9470,28 @@
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="9"/>
-      <c r="B6" s="140" t="s">
+      <c r="B6" s="106" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="108">
+        <v>314.25</v>
+      </c>
+      <c r="D6" s="106" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="109">
+        <v>42005</v>
+      </c>
+      <c r="F6" s="106" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="142">
-        <v>314.25</v>
-      </c>
-      <c r="D6" s="140" t="s">
+      <c r="G6" s="108">
+        <v>94443.520000000004</v>
+      </c>
+      <c r="H6" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="143">
-        <v>42005</v>
-      </c>
-      <c r="F6" s="140" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="142">
-        <v>94443.520000000004</v>
-      </c>
-      <c r="H6" s="140" t="s">
-        <v>72</v>
-      </c>
-      <c r="I6" s="143">
+      <c r="I6" s="109">
         <v>45658</v>
       </c>
       <c r="J6" s="17"/>

</xml_diff>